<commit_message>
Data Based SkillComponent works
</commit_message>
<xml_diff>
--- a/GameData/ABCharacterStatTable.xlsx
+++ b/GameData/ABCharacterStatTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeong\Desktop\UE5\ArenaBattle\GameData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF37188-E178-4685-BF7B-5BF90F04366C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7FA10D-11E4-4792-8947-0837548BFF67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="5565" windowWidth="20925" windowHeight="11595" xr2:uid="{14535CBB-5647-4022-885E-3A0FC95BEC4B}"/>
+    <workbookView xWindow="1365" yWindow="2340" windowWidth="20925" windowHeight="11595" xr2:uid="{14535CBB-5647-4022-885E-3A0FC95BEC4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Player" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Attack</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -78,6 +78,10 @@
   </si>
   <si>
     <t>AttackSpeedRate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AttackRangeForward</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -445,20 +449,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3D538BA-27C2-42AB-99FE-D911400E397E}">
-  <dimension ref="A2:F12"/>
+  <dimension ref="A2:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.875" style="1"/>
-    <col min="4" max="5" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -469,16 +473,19 @@
         <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -489,16 +496,19 @@
         <v>100</v>
       </c>
       <c r="D3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" s="1">
         <v>1</v>
       </c>
       <c r="F3" s="1">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -509,16 +519,19 @@
         <v>120</v>
       </c>
       <c r="D4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
         <v>1.05</v>
       </c>
-      <c r="F4" s="1">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -529,16 +542,19 @@
         <v>140</v>
       </c>
       <c r="D5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F5" s="1">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G5" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -549,16 +565,19 @@
         <v>160</v>
       </c>
       <c r="D6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
         <v>1.1499999999999999</v>
       </c>
-      <c r="F6" s="1">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G6" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -569,16 +588,19 @@
         <v>180</v>
       </c>
       <c r="D7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
         <v>1.2</v>
       </c>
-      <c r="F7" s="1">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G7" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -589,16 +611,19 @@
         <v>200</v>
       </c>
       <c r="D8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
         <v>1.25</v>
       </c>
-      <c r="F8" s="1">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G8" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -609,16 +634,19 @@
         <v>220</v>
       </c>
       <c r="D9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1">
         <v>1.3</v>
       </c>
-      <c r="F9" s="1">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G9" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -629,16 +657,19 @@
         <v>240</v>
       </c>
       <c r="D10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
         <v>1.35</v>
       </c>
-      <c r="F10" s="1">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G10" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -649,16 +680,19 @@
         <v>260</v>
       </c>
       <c r="D11" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" s="1">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1">
         <v>1.4</v>
       </c>
-      <c r="F11" s="1">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G11" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -669,12 +703,15 @@
         <v>280</v>
       </c>
       <c r="D12" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
         <v>1.45</v>
       </c>
-      <c r="F12" s="1">
+      <c r="G12" s="1">
         <v>400</v>
       </c>
     </row>

</xml_diff>

<commit_message>
rebalancing NPC Level Stat Table HpBar : Add Text for display current / max GimmickStage : Spawsn Opponents in random position
</commit_message>
<xml_diff>
--- a/GameData/ABCharacterStatTable.xlsx
+++ b/GameData/ABCharacterStatTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeong\Desktop\UE5\ArenaBattle\GameData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7FA10D-11E4-4792-8947-0837548BFF67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FC6BE01-4C9B-4F56-8F18-7CB24FF2DEF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1365" yWindow="2340" windowWidth="20925" windowHeight="11595" xr2:uid="{14535CBB-5647-4022-885E-3A0FC95BEC4B}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="28800" windowHeight="15345" xr2:uid="{14535CBB-5647-4022-885E-3A0FC95BEC4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Player" sheetId="2" r:id="rId1"/>
@@ -452,7 +452,7 @@
   <dimension ref="A2:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -493,7 +493,7 @@
         <v>100</v>
       </c>
       <c r="C3" s="1">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="D3" s="1">
         <v>0</v>
@@ -513,10 +513,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="1">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="C4" s="1">
-        <v>120</v>
+        <v>50</v>
       </c>
       <c r="D4" s="1">
         <v>0</v>
@@ -536,10 +536,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="1">
-        <v>200</v>
+        <v>160</v>
       </c>
       <c r="C5" s="1">
-        <v>140</v>
+        <v>75</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>
@@ -559,13 +559,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="1">
-        <v>250</v>
+        <v>190</v>
       </c>
       <c r="C6" s="1">
-        <v>160</v>
+        <v>115</v>
       </c>
       <c r="D6" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E6" s="1">
         <v>1</v>
@@ -582,13 +582,13 @@
         <v>7</v>
       </c>
       <c r="B7" s="1">
-        <v>300</v>
+        <v>230</v>
       </c>
       <c r="C7" s="1">
-        <v>180</v>
+        <v>155</v>
       </c>
       <c r="D7" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E7" s="1">
         <v>1</v>
@@ -597,7 +597,7 @@
         <v>1.2</v>
       </c>
       <c r="G7" s="1">
-        <v>400</v>
+        <v>480</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -605,13 +605,13 @@
         <v>8</v>
       </c>
       <c r="B8" s="1">
-        <v>350</v>
+        <v>330</v>
       </c>
       <c r="C8" s="1">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="D8" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E8" s="1">
         <v>1</v>
@@ -620,7 +620,7 @@
         <v>1.25</v>
       </c>
       <c r="G8" s="1">
-        <v>400</v>
+        <v>480</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -628,13 +628,13 @@
         <v>9</v>
       </c>
       <c r="B9" s="1">
-        <v>400</v>
+        <v>460</v>
       </c>
       <c r="C9" s="1">
-        <v>220</v>
+        <v>245</v>
       </c>
       <c r="D9" s="1">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E9" s="1">
         <v>1</v>
@@ -643,7 +643,7 @@
         <v>1.3</v>
       </c>
       <c r="G9" s="1">
-        <v>400</v>
+        <v>480</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -651,13 +651,13 @@
         <v>10</v>
       </c>
       <c r="B10" s="1">
-        <v>450</v>
+        <v>590</v>
       </c>
       <c r="C10" s="1">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="D10" s="1">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E10" s="1">
         <v>1</v>
@@ -666,7 +666,7 @@
         <v>1.35</v>
       </c>
       <c r="G10" s="1">
-        <v>400</v>
+        <v>560</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -674,13 +674,13 @@
         <v>11</v>
       </c>
       <c r="B11" s="1">
-        <v>500</v>
+        <v>720</v>
       </c>
       <c r="C11" s="1">
         <v>260</v>
       </c>
       <c r="D11" s="1">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E11" s="1">
         <v>1</v>
@@ -689,7 +689,7 @@
         <v>1.4</v>
       </c>
       <c r="G11" s="1">
-        <v>400</v>
+        <v>560</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -697,13 +697,13 @@
         <v>12</v>
       </c>
       <c r="B12" s="1">
-        <v>550</v>
+        <v>800</v>
       </c>
       <c r="C12" s="1">
-        <v>280</v>
+        <v>290</v>
       </c>
       <c r="D12" s="1">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E12" s="1">
         <v>1</v>
@@ -712,7 +712,7 @@
         <v>1.45</v>
       </c>
       <c r="G12" s="1">
-        <v>400</v>
+        <v>600</v>
       </c>
     </row>
   </sheetData>

</xml_diff>